<commit_message>
Updated Burndown chart, added scores and question number to trivia games
Trivia: Add scores and question numbers
Burndown Chart: Updated
</commit_message>
<xml_diff>
--- a/Trivia/Burndown.xlsx
+++ b/Trivia/Burndown.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Days</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>End Scrum 3</t>
-  </si>
-  <si>
-    <t>Start</t>
   </si>
 </sst>
 </file>
@@ -414,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -432,57 +429,49 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
         <v>0</v>
       </c>
     </row>

</xml_diff>